<commit_message>
Updates to config and Excel
</commit_message>
<xml_diff>
--- a/Hardware/Main Board/BOM LCSC.xlsx
+++ b/Hardware/Main Board/BOM LCSC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma Board\Hardware\Main Board\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Firmware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABF0FA4-8E4E-4FF2-B147-8B9EBA0814FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B373BE00-2BBF-4B7F-9E70-8789C4E5D1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="8775" windowWidth="35940" windowHeight="25485" activeTab="2" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="448">
   <si>
     <t>Package</t>
   </si>
@@ -633,9 +633,6 @@
     <t>Go</t>
   </si>
   <si>
-    <t>G4 Dwell or GRBL hold pin pulse high pulse from Torch to Grbl</t>
-  </si>
-  <si>
     <t>Handover</t>
   </si>
   <si>
@@ -645,9 +642,6 @@
     <t>TorchReady</t>
   </si>
   <si>
-    <t>Pulse to Grbl to Go</t>
-  </si>
-  <si>
     <t>Climit   36</t>
   </si>
   <si>
@@ -1351,6 +1345,60 @@
   </si>
   <si>
     <t>Optocoupler</t>
+  </si>
+  <si>
+    <t>GPIO 2</t>
+  </si>
+  <si>
+    <t>GPIO 25</t>
+  </si>
+  <si>
+    <t>GPIO 39</t>
+  </si>
+  <si>
+    <t>B Limit</t>
+  </si>
+  <si>
+    <t>GPIO 36</t>
+  </si>
+  <si>
+    <t>C Limit</t>
+  </si>
+  <si>
+    <t>GPIO 14</t>
+  </si>
+  <si>
+    <t>GPIO 13</t>
+  </si>
+  <si>
+    <t>Module 2</t>
+  </si>
+  <si>
+    <t>Module 1</t>
+  </si>
+  <si>
+    <t>J1-J4 Juper</t>
+  </si>
+  <si>
+    <t>G4 Dwell or GRBL hold pin pulse low pulse from Torch to Grbl</t>
+  </si>
+  <si>
+    <t>Low pulse</t>
+  </si>
+  <si>
+    <t>Pulse low to Grbl to Go</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>Macro 0</t>
+  </si>
+  <si>
+    <t>Macro1</t>
+  </si>
+  <si>
+    <t>Macro 2</t>
   </si>
 </sst>
 </file>
@@ -3030,8 +3078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C39F3-7594-4535-810B-0496FC455A11}">
   <dimension ref="B1:O96"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="L82" sqref="L82"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="N68" sqref="N68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3102,16 +3150,16 @@
         <v>161</v>
       </c>
       <c r="K4" s="17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="L4" s="17" t="s">
         <v>23</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O4" s="17"/>
     </row>
@@ -3203,7 +3251,7 @@
         <v>158</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D10">
         <v>26</v>
@@ -3264,13 +3312,13 @@
     </row>
     <row r="12" spans="2:15">
       <c r="B12" t="s">
-        <v>192</v>
+        <v>441</v>
       </c>
       <c r="C12" t="s">
         <v>189</v>
       </c>
       <c r="D12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E12">
         <v>33</v>
@@ -3279,7 +3327,7 @@
         <v>146</v>
       </c>
       <c r="G12" t="s">
-        <v>148</v>
+        <v>442</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>191</v>
@@ -3328,10 +3376,10 @@
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C14" t="s">
         <v>194</v>
-      </c>
-      <c r="C14" t="s">
-        <v>195</v>
       </c>
       <c r="E14">
         <v>14</v>
@@ -3353,19 +3401,22 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
+        <v>443</v>
+      </c>
+      <c r="C15" t="s">
         <v>196</v>
       </c>
-      <c r="C15" t="s">
-        <v>198</v>
-      </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E15">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>200</v>
+        <v>198</v>
+      </c>
+      <c r="G15" t="s">
+        <v>442</v>
       </c>
       <c r="I15" s="19"/>
       <c r="J15" s="20"/>
@@ -3379,10 +3430,10 @@
     </row>
     <row r="16" spans="2:15">
       <c r="B16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J16" s="20">
         <v>1</v>
@@ -3399,7 +3450,7 @@
     </row>
     <row r="17" spans="2:15">
       <c r="B17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I17" s="19"/>
       <c r="J17" s="20">
@@ -3435,7 +3486,7 @@
     </row>
     <row r="19" spans="2:15">
       <c r="B19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E19">
         <v>32</v>
@@ -3459,7 +3510,7 @@
     </row>
     <row r="20" spans="2:15">
       <c r="B20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E20">
         <v>19</v>
@@ -3479,7 +3530,7 @@
     </row>
     <row r="21" spans="2:15">
       <c r="B21" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I21" s="19"/>
       <c r="J21" s="20">
@@ -3511,7 +3562,7 @@
     </row>
     <row r="23" spans="2:15">
       <c r="B23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I23" s="19" t="s">
         <v>191</v>
@@ -3540,7 +3591,7 @@
     </row>
     <row r="25" spans="2:15">
       <c r="I25" s="19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J25" s="20">
         <v>1</v>
@@ -3585,14 +3636,14 @@
         <v>4</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="19" t="s">
         <v>174</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O28" s="17"/>
     </row>
@@ -3643,12 +3694,12 @@
         <v>8</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
       <c r="N32" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="O32" s="17"/>
     </row>
@@ -3658,14 +3709,14 @@
         <v>9</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L33" s="19"/>
       <c r="M33" s="19" t="s">
         <v>174</v>
       </c>
       <c r="N33" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O33" s="17"/>
     </row>
@@ -3680,7 +3731,7 @@
       <c r="L34" s="19"/>
       <c r="M34" s="19"/>
       <c r="N34" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="O34" s="17"/>
     </row>
@@ -3732,7 +3783,7 @@
     </row>
     <row r="39" spans="9:15">
       <c r="I39" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J39" s="22">
         <v>1</v>
@@ -3751,7 +3802,7 @@
         <v>2</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
@@ -3777,7 +3828,7 @@
         <v>4</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="L42" s="21"/>
       <c r="M42" s="21"/>
@@ -3803,7 +3854,7 @@
         <v>6</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="L44" s="21"/>
       <c r="M44" s="21"/>
@@ -3829,7 +3880,7 @@
         <v>8</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
@@ -3842,7 +3893,7 @@
         <v>9</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L47" s="21"/>
       <c r="M47" s="21"/>
@@ -3855,7 +3906,7 @@
         <v>10</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
@@ -3873,7 +3924,7 @@
     </row>
     <row r="50" spans="9:15">
       <c r="I50" s="23" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J50" s="24">
         <v>1</v>
@@ -3887,15 +3938,17 @@
       <c r="O50" s="17"/>
     </row>
     <row r="51" spans="9:15">
-      <c r="I51" s="23"/>
+      <c r="I51" s="23" t="s">
+        <v>439</v>
+      </c>
       <c r="J51" s="24">
         <v>2</v>
       </c>
       <c r="K51" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="L51" s="23" t="s">
         <v>217</v>
-      </c>
-      <c r="L51" s="23" t="s">
-        <v>219</v>
       </c>
       <c r="M51" s="23"/>
       <c r="N51" s="23"/>
@@ -3923,7 +3976,7 @@
         <v>141</v>
       </c>
       <c r="L53" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="M53" s="23"/>
       <c r="N53" s="23"/>
@@ -3932,10 +3985,10 @@
     <row r="54" spans="9:15">
       <c r="I54" s="23"/>
       <c r="J54" s="24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K54" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L54" s="23"/>
       <c r="M54" s="23"/>
@@ -3953,7 +4006,7 @@
     </row>
     <row r="56" spans="9:15">
       <c r="I56" s="23" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J56" s="24">
         <v>1</v>
@@ -3985,7 +4038,7 @@
         <v>6</v>
       </c>
       <c r="K58" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L58" s="23"/>
       <c r="M58" s="23"/>
@@ -3998,7 +4051,7 @@
         <v>7</v>
       </c>
       <c r="K59" s="23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L59" s="23"/>
       <c r="M59" s="23"/>
@@ -4029,13 +4082,13 @@
     </row>
     <row r="62" spans="9:15">
       <c r="I62" s="25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J62" s="26">
         <v>1</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L62" s="25"/>
       <c r="M62" s="25"/>
@@ -4043,16 +4096,22 @@
       <c r="O62" s="17"/>
     </row>
     <row r="63" spans="9:15">
-      <c r="I63" s="25"/>
+      <c r="I63" s="25" t="s">
+        <v>438</v>
+      </c>
       <c r="J63" s="26">
         <v>2</v>
       </c>
       <c r="K63" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="L63" s="25"/>
+        <v>227</v>
+      </c>
+      <c r="L63" s="25" t="s">
+        <v>430</v>
+      </c>
       <c r="M63" s="25"/>
-      <c r="N63" s="25"/>
+      <c r="N63" s="25" t="s">
+        <v>444</v>
+      </c>
       <c r="O63" s="17"/>
     </row>
     <row r="64" spans="9:15">
@@ -4061,11 +4120,15 @@
         <v>3</v>
       </c>
       <c r="K64" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="L64" s="25"/>
+        <v>228</v>
+      </c>
+      <c r="L64" s="25" t="s">
+        <v>431</v>
+      </c>
       <c r="M64" s="25"/>
-      <c r="N64" s="25"/>
+      <c r="N64" s="25" t="s">
+        <v>445</v>
+      </c>
       <c r="O64" s="17"/>
     </row>
     <row r="65" spans="2:15">
@@ -4077,11 +4140,17 @@
         <v>4</v>
       </c>
       <c r="K65" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="L65" s="25"/>
-      <c r="M65" s="25"/>
-      <c r="N65" s="25"/>
+        <v>229</v>
+      </c>
+      <c r="L65" s="25" t="s">
+        <v>432</v>
+      </c>
+      <c r="M65" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="N65" s="25" t="s">
+        <v>190</v>
+      </c>
       <c r="O65" s="17"/>
     </row>
     <row r="66" spans="2:15">
@@ -4090,11 +4159,17 @@
         <v>5</v>
       </c>
       <c r="K66" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="L66" s="25"/>
-      <c r="M66" s="25"/>
-      <c r="N66" s="25"/>
+        <v>230</v>
+      </c>
+      <c r="L66" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="M66" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="N66" s="25" t="s">
+        <v>139</v>
+      </c>
       <c r="O66" s="17"/>
     </row>
     <row r="67" spans="2:15">
@@ -4103,11 +4178,15 @@
         <v>6</v>
       </c>
       <c r="K67" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="L67" s="25"/>
+        <v>231</v>
+      </c>
+      <c r="L67" s="25" t="s">
+        <v>436</v>
+      </c>
       <c r="M67" s="25"/>
-      <c r="N67" s="25"/>
+      <c r="N67" s="25" t="s">
+        <v>446</v>
+      </c>
       <c r="O67" s="17"/>
     </row>
     <row r="68" spans="2:15">
@@ -4116,11 +4195,15 @@
         <v>7</v>
       </c>
       <c r="K68" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="L68" s="25"/>
+        <v>232</v>
+      </c>
+      <c r="L68" s="25" t="s">
+        <v>437</v>
+      </c>
       <c r="M68" s="25"/>
-      <c r="N68" s="25"/>
+      <c r="N68" s="25" t="s">
+        <v>447</v>
+      </c>
       <c r="O68" s="17"/>
     </row>
     <row r="69" spans="2:15">
@@ -4129,7 +4212,7 @@
         <v>8</v>
       </c>
       <c r="K69" s="25" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L69" s="25"/>
       <c r="M69" s="25"/>
@@ -4147,7 +4230,7 @@
     </row>
     <row r="71" spans="2:15">
       <c r="I71" s="25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J71" s="26">
         <v>1</v>
@@ -4156,7 +4239,7 @@
         <v>21</v>
       </c>
       <c r="L71" s="25" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M71" s="25"/>
       <c r="N71" s="25"/>
@@ -4168,10 +4251,10 @@
         <v>2</v>
       </c>
       <c r="K72" s="25" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L72" s="25" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M72" s="25"/>
       <c r="N72" s="25"/>
@@ -4183,10 +4266,10 @@
         <v>3</v>
       </c>
       <c r="K73" s="25" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L73" s="25" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M73" s="25"/>
       <c r="N73" s="25"/>
@@ -4198,10 +4281,10 @@
         <v>4</v>
       </c>
       <c r="K74" s="25" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L74" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="M74" s="25"/>
       <c r="N74" s="25"/>
@@ -4213,10 +4296,10 @@
         <v>5</v>
       </c>
       <c r="K75" s="25" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L75" s="25" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M75" s="25"/>
       <c r="N75" s="25"/>
@@ -4228,10 +4311,10 @@
         <v>6</v>
       </c>
       <c r="K76" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L76" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M76" s="25"/>
       <c r="N76" s="25"/>
@@ -4243,10 +4326,10 @@
         <v>8</v>
       </c>
       <c r="K77" s="25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L77" s="25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M77" s="25"/>
       <c r="N77" s="25"/>
@@ -4258,10 +4341,10 @@
         <v>9</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L78" s="25" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M78" s="25"/>
       <c r="N78" s="25"/>
@@ -4269,16 +4352,16 @@
     </row>
     <row r="79" spans="2:15">
       <c r="I79" s="17" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J79" s="18">
         <v>1</v>
       </c>
       <c r="K79" s="17" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L79" s="17" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M79" s="17"/>
       <c r="N79" s="17"/>
@@ -4290,10 +4373,10 @@
         <v>2</v>
       </c>
       <c r="K80" s="17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="L80" s="17" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M80" s="17"/>
       <c r="N80" s="17"/>
@@ -4301,13 +4384,13 @@
     </row>
     <row r="81" spans="9:15">
       <c r="I81" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J81" s="15">
         <v>1</v>
       </c>
       <c r="K81" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="O81" s="17"/>
     </row>
@@ -4316,12 +4399,12 @@
         <v>2</v>
       </c>
       <c r="K82" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="85" spans="9:15">
       <c r="I85" s="27" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J85" s="28">
         <v>1</v>
@@ -4330,12 +4413,12 @@
       <c r="L85" s="27"/>
       <c r="M85" s="27"/>
       <c r="N85" s="27" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="86" spans="9:15">
       <c r="I86" s="27" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J86" s="28">
         <v>2</v>
@@ -4356,7 +4439,7 @@
       <c r="L87" s="29"/>
       <c r="M87" s="29"/>
       <c r="N87" s="29" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="88" spans="9:15">
@@ -4365,9 +4448,11 @@
         <v>4</v>
       </c>
       <c r="K88" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="L88" s="29"/>
+        <v>271</v>
+      </c>
+      <c r="L88" s="29" t="s">
+        <v>440</v>
+      </c>
       <c r="M88" s="29"/>
       <c r="N88" s="27" t="s">
         <v>169</v>
@@ -4379,12 +4464,14 @@
         <v>5</v>
       </c>
       <c r="K89" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="L89" s="29"/>
+        <v>270</v>
+      </c>
+      <c r="L89" s="29" t="s">
+        <v>440</v>
+      </c>
       <c r="M89" s="29"/>
       <c r="N89" s="27" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="90" spans="9:15">
@@ -4393,12 +4480,14 @@
         <v>6</v>
       </c>
       <c r="K90" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="L90" s="29"/>
+        <v>269</v>
+      </c>
+      <c r="L90" s="29" t="s">
+        <v>440</v>
+      </c>
       <c r="M90" s="29"/>
       <c r="N90" s="27" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="91" spans="9:15">
@@ -4407,12 +4496,14 @@
         <v>7</v>
       </c>
       <c r="K91" s="29" t="s">
-        <v>270</v>
-      </c>
-      <c r="L91" s="29"/>
+        <v>268</v>
+      </c>
+      <c r="L91" s="29" t="s">
+        <v>440</v>
+      </c>
       <c r="M91" s="29"/>
       <c r="N91" s="27" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="92" spans="9:15">
@@ -4421,12 +4512,12 @@
         <v>8</v>
       </c>
       <c r="K92" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L92" s="29"/>
       <c r="M92" s="29"/>
       <c r="N92" s="27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="93" spans="9:15">
@@ -4435,12 +4526,12 @@
         <v>9</v>
       </c>
       <c r="K93" s="29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L93" s="29"/>
       <c r="M93" s="29"/>
       <c r="N93" s="27" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="94" spans="9:15">
@@ -4449,7 +4540,7 @@
         <v>10</v>
       </c>
       <c r="K94" s="29" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L94" s="29"/>
       <c r="M94" s="29"/>
@@ -4463,7 +4554,7 @@
         <v>11</v>
       </c>
       <c r="K95" s="29" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L95" s="29"/>
       <c r="M95" s="29"/>
@@ -4480,7 +4571,7 @@
       <c r="L96" s="29"/>
       <c r="M96" s="29"/>
       <c r="N96" s="27" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -4497,7 +4588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CF0671-FE26-4F07-89AC-F4C1AA2B534B}">
   <dimension ref="A2:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -5193,8 +5284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B019C195-3E7A-4EF2-BB4B-1128AF09E9D2}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5211,7 +5302,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B1" t="s">
         <v>56</v>
@@ -5220,19 +5311,19 @@
         <v>58</v>
       </c>
       <c r="D1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F1" t="s">
         <v>333</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>334</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>335</v>
-      </c>
-      <c r="G1" t="s">
-        <v>336</v>
-      </c>
-      <c r="H1" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -5240,22 +5331,22 @@
         <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C2">
         <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="G2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H2">
         <v>16</v>
@@ -5263,19 +5354,19 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F3" t="s">
         <v>102</v>
@@ -5289,19 +5380,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F4" t="s">
         <v>89</v>
@@ -5318,22 +5409,22 @@
         <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E5" t="s">
+        <v>354</v>
+      </c>
+      <c r="F5" t="s">
+        <v>355</v>
+      </c>
+      <c r="G5" t="s">
         <v>356</v>
-      </c>
-      <c r="F5" t="s">
-        <v>357</v>
-      </c>
-      <c r="G5" t="s">
-        <v>358</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -5341,22 +5432,22 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H6">
         <v>4</v>
@@ -5367,22 +5458,22 @@
         <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H7">
         <v>8</v>
@@ -5390,19 +5481,19 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E8" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F8" t="s">
         <v>87</v>
@@ -5416,25 +5507,25 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B9" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F9" t="s">
         <v>300</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>301</v>
-      </c>
-      <c r="F9" t="s">
-        <v>302</v>
-      </c>
-      <c r="G9" t="s">
-        <v>303</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -5442,22 +5533,22 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C10" t="s">
         <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F10" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H10">
         <v>8</v>
@@ -5468,22 +5559,22 @@
         <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D11" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F11" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G11" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H11">
         <v>8</v>
@@ -5494,22 +5585,22 @@
         <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E12" t="s">
+        <v>367</v>
+      </c>
+      <c r="F12" t="s">
+        <v>368</v>
+      </c>
+      <c r="G12" t="s">
         <v>369</v>
-      </c>
-      <c r="F12" t="s">
-        <v>370</v>
-      </c>
-      <c r="G12" t="s">
-        <v>371</v>
       </c>
       <c r="H12">
         <v>5</v>
@@ -5517,16 +5608,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H13">
         <v>6</v>
@@ -5534,16 +5625,16 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H14">
         <v>6</v>
@@ -5551,16 +5642,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H15">
         <v>12</v>
@@ -5571,22 +5662,22 @@
         <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C16" t="s">
+        <v>395</v>
+      </c>
+      <c r="D16" t="s">
+        <v>316</v>
+      </c>
+      <c r="E16" t="s">
+        <v>296</v>
+      </c>
+      <c r="F16" t="s">
+        <v>396</v>
+      </c>
+      <c r="G16" t="s">
         <v>397</v>
-      </c>
-      <c r="D16" t="s">
-        <v>318</v>
-      </c>
-      <c r="E16" t="s">
-        <v>298</v>
-      </c>
-      <c r="F16" t="s">
-        <v>398</v>
-      </c>
-      <c r="G16" t="s">
-        <v>399</v>
       </c>
       <c r="H16">
         <v>4</v>
@@ -5597,22 +5688,22 @@
         <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C17" t="s">
+        <v>361</v>
+      </c>
+      <c r="D17" t="s">
+        <v>287</v>
+      </c>
+      <c r="E17" t="s">
+        <v>362</v>
+      </c>
+      <c r="F17" t="s">
         <v>363</v>
       </c>
-      <c r="D17" t="s">
-        <v>289</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>364</v>
-      </c>
-      <c r="F17" t="s">
-        <v>365</v>
-      </c>
-      <c r="G17" t="s">
-        <v>366</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -5620,19 +5711,19 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B18" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F18" t="s">
         <v>104</v>
@@ -5649,22 +5740,22 @@
         <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C19" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D19" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F19" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G19" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -5672,16 +5763,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
+        <v>337</v>
+      </c>
+      <c r="B20" t="s">
         <v>339</v>
       </c>
-      <c r="B20" t="s">
-        <v>341</v>
-      </c>
       <c r="C20" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H20">
         <v>6</v>
@@ -5689,16 +5780,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B21" t="s">
+        <v>350</v>
+      </c>
+      <c r="C21" t="s">
+        <v>351</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>352</v>
-      </c>
-      <c r="C21" t="s">
-        <v>353</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>354</v>
       </c>
       <c r="H21">
         <v>6</v>
@@ -5709,22 +5800,22 @@
         <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C22" t="s">
+        <v>392</v>
+      </c>
+      <c r="D22" t="s">
+        <v>316</v>
+      </c>
+      <c r="E22" t="s">
+        <v>296</v>
+      </c>
+      <c r="F22" t="s">
+        <v>393</v>
+      </c>
+      <c r="G22" t="s">
         <v>394</v>
-      </c>
-      <c r="D22" t="s">
-        <v>318</v>
-      </c>
-      <c r="E22" t="s">
-        <v>298</v>
-      </c>
-      <c r="F22" t="s">
-        <v>395</v>
-      </c>
-      <c r="G22" t="s">
-        <v>396</v>
       </c>
       <c r="H22">
         <v>4</v>
@@ -5732,25 +5823,25 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B23" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
       </c>
       <c r="D23" t="s">
+        <v>298</v>
+      </c>
+      <c r="E23" t="s">
+        <v>299</v>
+      </c>
+      <c r="F23" t="s">
         <v>300</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>301</v>
-      </c>
-      <c r="F23" t="s">
-        <v>302</v>
-      </c>
-      <c r="G23" t="s">
-        <v>303</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -5758,19 +5849,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B24" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F24" t="s">
         <v>91</v>
@@ -5784,25 +5875,25 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B25" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
       <c r="D25" t="s">
+        <v>298</v>
+      </c>
+      <c r="E25" t="s">
+        <v>299</v>
+      </c>
+      <c r="F25" t="s">
         <v>300</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>301</v>
-      </c>
-      <c r="F25" t="s">
-        <v>302</v>
-      </c>
-      <c r="G25" t="s">
-        <v>303</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -5810,19 +5901,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B26" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C26" t="s">
         <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E26" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F26" t="s">
         <v>116</v>
@@ -5836,19 +5927,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B27" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C27" t="s">
         <v>48</v>
       </c>
       <c r="D27" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E27" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F27" t="s">
         <v>112</v>
@@ -5868,19 +5959,19 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
+        <v>386</v>
+      </c>
+      <c r="D28" t="s">
+        <v>387</v>
+      </c>
+      <c r="E28" t="s">
         <v>388</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>389</v>
       </c>
-      <c r="E28" t="s">
-        <v>390</v>
-      </c>
-      <c r="F28" t="s">
-        <v>391</v>
-      </c>
       <c r="G28" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -5891,22 +5982,22 @@
         <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C29" t="s">
+        <v>370</v>
+      </c>
+      <c r="D29" t="s">
+        <v>371</v>
+      </c>
+      <c r="E29" t="s">
         <v>372</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>373</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>374</v>
-      </c>
-      <c r="F29" t="s">
-        <v>375</v>
-      </c>
-      <c r="G29" t="s">
-        <v>376</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -5914,19 +6005,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B30" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E30" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F30" t="s">
         <v>93</v>
@@ -5940,25 +6031,25 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B31" t="s">
+        <v>323</v>
+      </c>
+      <c r="C31" t="s">
+        <v>324</v>
+      </c>
+      <c r="D31" t="s">
         <v>325</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>326</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>327</v>
       </c>
-      <c r="E31" t="s">
-        <v>328</v>
-      </c>
-      <c r="F31" t="s">
-        <v>329</v>
-      </c>
       <c r="G31" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="H31">
         <v>1</v>
@@ -5969,22 +6060,22 @@
         <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C32" t="s">
+        <v>375</v>
+      </c>
+      <c r="D32" t="s">
+        <v>316</v>
+      </c>
+      <c r="E32" t="s">
+        <v>376</v>
+      </c>
+      <c r="F32" t="s">
         <v>377</v>
       </c>
-      <c r="D32" t="s">
-        <v>318</v>
-      </c>
-      <c r="E32" t="s">
-        <v>378</v>
-      </c>
-      <c r="F32" t="s">
-        <v>379</v>
-      </c>
       <c r="G32" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -6001,10 +6092,10 @@
         <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E33" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F33" t="s">
         <v>100</v>
@@ -6018,19 +6109,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B34" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C34" t="s">
         <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E34" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F34" t="s">
         <v>102</v>
@@ -6053,10 +6144,10 @@
         <v>74</v>
       </c>
       <c r="D35" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E35" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F35" t="s">
         <v>118</v>
@@ -6073,22 +6164,22 @@
         <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D36" t="s">
+        <v>357</v>
+      </c>
+      <c r="E36" t="s">
+        <v>358</v>
+      </c>
+      <c r="F36" t="s">
         <v>359</v>
       </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
         <v>360</v>
-      </c>
-      <c r="F36" t="s">
-        <v>361</v>
-      </c>
-      <c r="G36" t="s">
-        <v>362</v>
       </c>
       <c r="H36">
         <v>5</v>
@@ -6099,22 +6190,22 @@
         <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C37" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D37" t="s">
+        <v>398</v>
+      </c>
+      <c r="E37" t="s">
+        <v>399</v>
+      </c>
+      <c r="F37" t="s">
         <v>400</v>
       </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>401</v>
-      </c>
-      <c r="F37" t="s">
-        <v>402</v>
-      </c>
-      <c r="G37" t="s">
-        <v>403</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -6122,19 +6213,19 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B38" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C38" t="s">
         <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E38" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F38" t="s">
         <v>123</v>
@@ -6151,16 +6242,16 @@
         <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C39" t="s">
         <v>94</v>
       </c>
       <c r="D39" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E39" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F39" t="s">
         <v>93</v>
@@ -6180,19 +6271,19 @@
         <v>46</v>
       </c>
       <c r="C40" t="s">
+        <v>404</v>
+      </c>
+      <c r="D40" t="s">
+        <v>405</v>
+      </c>
+      <c r="E40" t="s">
         <v>406</v>
       </c>
-      <c r="D40" t="s">
+      <c r="F40" t="s">
         <v>407</v>
       </c>
-      <c r="E40" t="s">
-        <v>408</v>
-      </c>
-      <c r="F40" t="s">
-        <v>409</v>
-      </c>
       <c r="G40" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -6203,22 +6294,22 @@
         <v>84</v>
       </c>
       <c r="B41" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C41" t="s">
         <v>62</v>
       </c>
       <c r="D41" t="s">
+        <v>398</v>
+      </c>
+      <c r="E41" t="s">
+        <v>399</v>
+      </c>
+      <c r="F41" t="s">
         <v>400</v>
       </c>
-      <c r="E41" t="s">
+      <c r="G41" t="s">
         <v>401</v>
-      </c>
-      <c r="F41" t="s">
-        <v>402</v>
-      </c>
-      <c r="G41" t="s">
-        <v>403</v>
       </c>
       <c r="H41">
         <v>2</v>
@@ -6235,16 +6326,16 @@
         <v>83</v>
       </c>
       <c r="D42" t="s">
+        <v>378</v>
+      </c>
+      <c r="E42" t="s">
+        <v>379</v>
+      </c>
+      <c r="F42" t="s">
         <v>380</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42" t="s">
         <v>381</v>
-      </c>
-      <c r="F42" t="s">
-        <v>382</v>
-      </c>
-      <c r="G42" t="s">
-        <v>383</v>
       </c>
       <c r="H42">
         <v>1</v>
@@ -6252,25 +6343,25 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B43" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C43" t="s">
         <v>15</v>
       </c>
       <c r="D43" t="s">
+        <v>298</v>
+      </c>
+      <c r="E43" t="s">
+        <v>299</v>
+      </c>
+      <c r="F43" t="s">
         <v>300</v>
       </c>
-      <c r="E43" t="s">
+      <c r="G43" t="s">
         <v>301</v>
-      </c>
-      <c r="F43" t="s">
-        <v>302</v>
-      </c>
-      <c r="G43" t="s">
-        <v>303</v>
       </c>
       <c r="H43">
         <v>1</v>
@@ -6278,13 +6369,13 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B44" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F44" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H44">
         <v>1</v>
@@ -6340,10 +6431,10 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="2:3">
@@ -6429,7 +6520,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6680,7 +6771,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>4</v>
@@ -6692,10 +6783,10 @@
         <v>4</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K9">
         <v>20</v>
@@ -6872,16 +6963,16 @@
     </row>
     <row r="18" spans="3:11">
       <c r="C18" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E18" t="s">
+        <v>243</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="J18" s="11" t="s">
         <v>244</v>
-      </c>
-      <c r="E18" t="s">
-        <v>245</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>246</v>
       </c>
       <c r="K18">
         <v>20</v>
@@ -6889,16 +6980,16 @@
     </row>
     <row r="19" spans="3:11">
       <c r="C19" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" t="s">
+        <v>250</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J19" s="11" t="s">
         <v>251</v>
-      </c>
-      <c r="E19" t="s">
-        <v>252</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>253</v>
       </c>
       <c r="K19">
         <v>60</v>
@@ -6906,16 +6997,16 @@
     </row>
     <row r="20" spans="3:11">
       <c r="C20" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E20" t="s">
+        <v>253</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>257</v>
-      </c>
       <c r="J20" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K20">
         <v>50</v>

</xml_diff>

<commit_message>
added a test gcode file
added a test gcode file
</commit_message>
<xml_diff>
--- a/Hardware/Main Board/BOM LCSC.xlsx
+++ b/Hardware/Main Board/BOM LCSC.xlsx
@@ -5,25 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Firmware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Main Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B373BE00-2BBF-4B7F-9E70-8789C4E5D1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0920821D-2F4F-4BCD-9969-3B1AF50EB214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
-    <sheet name="BOM" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="Torch Module" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
+    <sheet name="Changes" sheetId="6" r:id="rId2"/>
+    <sheet name="test box" sheetId="7" r:id="rId3"/>
+    <sheet name="BOM" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Torch Module" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BOM!$A$2:$M$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet1!$A$1:$H$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BOM!$A$2:$M$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$A$1:$H$43</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Connectors!#REF!</definedName>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Torch Module'!#REF!</definedName>
+    <definedName name="ExternalData_1" localSheetId="5" hidden="1">'Torch Module'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="480">
   <si>
     <t>Package</t>
   </si>
@@ -1399,6 +1401,102 @@
   </si>
   <si>
     <t>Macro 2</t>
+  </si>
+  <si>
+    <t>Mainboard</t>
+  </si>
+  <si>
+    <t>U1 to J9</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>U1 Txd - J9 - 3</t>
+  </si>
+  <si>
+    <t>U1Rxd - J9 - 4</t>
+  </si>
+  <si>
+    <t>U1 17 - J9 - 3</t>
+  </si>
+  <si>
+    <t>U1 16 - J9 - 4</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>3.3v   -  J9 - 1</t>
+  </si>
+  <si>
+    <t>5v  -  J9 - 1</t>
+  </si>
+  <si>
+    <t>Torch Mod#3</t>
+  </si>
+  <si>
+    <t>RV1  100K</t>
+  </si>
+  <si>
+    <t>R3  33K</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>Torch control board Module 3</t>
+  </si>
+  <si>
+    <t>J15  invert 3 and 4 on silk screen</t>
+  </si>
+  <si>
+    <t>Mosfet motor driver</t>
+  </si>
+  <si>
+    <t>Source and Drain swaped on PCB board wrong foot print</t>
+  </si>
+  <si>
+    <t>Darlington Driver</t>
+  </si>
+  <si>
+    <t>ULN2002 needs 12 vto turn on Try ULN2003</t>
+  </si>
+  <si>
+    <t>Watch direction of D1</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>RJ45</t>
+  </si>
+  <si>
+    <t>Change serial port to Nexion so usb serial is free</t>
+  </si>
+  <si>
+    <t>RX 16</t>
+  </si>
+  <si>
+    <t>Tx 17</t>
+  </si>
+  <si>
+    <t>pin 1 on Thc displayJ( needs to be 5v not 3.3</t>
+  </si>
+  <si>
+    <t>switch Handover from GPIO12 to13 12 is a boot pin</t>
+  </si>
+  <si>
+    <t>Rj45 for J9 we ordered has magnetics</t>
+  </si>
+  <si>
+    <t>Motor driver too RJ45</t>
+  </si>
+  <si>
+    <t>mixed up when we changed connectors</t>
   </si>
 </sst>
 </file>
@@ -2725,6 +2823,79 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>200025</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>47624</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3073" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s3073"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B07AFE74-B9C0-427C-8216-867C4D2BD771}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd type="none" w="med" len="med"/>
+            </a:ln>
+            <a:effectLst/>
+            <a:extLst>
+              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
+                <a14:hiddenEffects>
+                  <a:effectLst>
+                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="808080"/>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </a14:hiddenEffects>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -3078,7 +3249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C39F3-7594-4535-810B-0496FC455A11}">
   <dimension ref="B1:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="N68" sqref="N68"/>
     </sheetView>
   </sheetViews>
@@ -4585,6 +4756,243 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E6E9A4-984E-47E0-AB78-3A5B51A2C28B}">
+  <dimension ref="A1:M21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="10" max="10" width="32.7109375" customWidth="1"/>
+    <col min="11" max="11" width="52.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="B2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="C3" t="s">
+        <v>455</v>
+      </c>
+      <c r="D3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C4" t="s">
+        <v>458</v>
+      </c>
+      <c r="D4" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="C5" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>463</v>
+      </c>
+      <c r="K6" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>459</v>
+      </c>
+      <c r="C7" t="s">
+        <v>460</v>
+      </c>
+      <c r="D7" t="s">
+        <v>462</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="C8" t="s">
+        <v>461</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="C9" t="s">
+        <v>464</v>
+      </c>
+      <c r="J9" t="s">
+        <v>465</v>
+      </c>
+      <c r="K9" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="J11" t="s">
+        <v>467</v>
+      </c>
+      <c r="K11" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>465</v>
+      </c>
+      <c r="B12" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="J13" t="s">
+        <v>448</v>
+      </c>
+      <c r="K13" t="s">
+        <v>469</v>
+      </c>
+      <c r="L13" t="s">
+        <v>470</v>
+      </c>
+      <c r="M13" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>467</v>
+      </c>
+      <c r="B14" t="s">
+        <v>468</v>
+      </c>
+      <c r="K14" t="s">
+        <v>472</v>
+      </c>
+      <c r="L14" t="s">
+        <v>473</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="L15" t="s">
+        <v>474</v>
+      </c>
+      <c r="M15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="K16" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11">
+      <c r="K17" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="19" spans="10:11">
+      <c r="K19" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="21" spans="10:11">
+      <c r="J21" t="s">
+        <v>478</v>
+      </c>
+      <c r="K21" t="s">
+        <v>479</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63752E21-50CB-4B23-8BB5-9505E3D6C816}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="3073" r:id="rId4">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>200025</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="3073" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CF0671-FE26-4F07-89AC-F4C1AA2B534B}">
   <dimension ref="A2:N20"/>
   <sheetViews>
@@ -5280,7 +5688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B019C195-3E7A-4EF2-BB4B-1128AF09E9D2}">
   <dimension ref="A1:H64"/>
   <sheetViews>
@@ -6409,7 +6817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192ADD7D-D55E-4CB1-B608-DE63AF189E80}">
   <dimension ref="B1:C10"/>
   <sheetViews>
@@ -6515,7 +6923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDEC5E0-5FF0-4FCF-B471-4DD68D399C1F}">
   <dimension ref="A1:M20"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Quad input and Output Modules
Input and Output modules
</commit_message>
<xml_diff>
--- a/Hardware/Main Board/BOM LCSC.xlsx
+++ b/Hardware/Main Board/BOM LCSC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Main Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0920821D-2F4F-4BCD-9969-3B1AF50EB214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9826999B-05B4-4628-B08A-FF4A576BDDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="12180" yWindow="5115" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="489">
   <si>
     <t>Package</t>
   </si>
@@ -1497,6 +1497,33 @@
   </si>
   <si>
     <t>mixed up when we changed connectors</t>
+  </si>
+  <si>
+    <t>Silk screen</t>
+  </si>
+  <si>
+    <t>Z Limit   to</t>
+  </si>
+  <si>
+    <t>J17 Reset</t>
+  </si>
+  <si>
+    <t>J17 Grbl Reset</t>
+  </si>
+  <si>
+    <t>J18 Reset</t>
+  </si>
+  <si>
+    <t>J18 Grbl Reset</t>
+  </si>
+  <si>
+    <t>Mod 1</t>
+  </si>
+  <si>
+    <t>Show polarity on J7 &amp;J8</t>
+  </si>
+  <si>
+    <t>Show voltages onD2,3,4,5</t>
   </si>
 </sst>
 </file>
@@ -2836,7 +2863,7 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>200025</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>47624</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2846,7 +2873,7 @@
                   <a14:compatExt spid="_x0000_s3073"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B07AFE74-B9C0-427C-8216-867C4D2BD771}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000010C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2867,23 +2894,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -4757,10 +4771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E6E9A4-984E-47E0-AB78-3A5B51A2C28B}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4925,22 +4939,59 @@
         <v>475</v>
       </c>
     </row>
-    <row r="17" spans="10:11">
+    <row r="17" spans="1:11">
       <c r="K17" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="19" spans="10:11">
+    <row r="19" spans="1:11">
       <c r="K19" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="21" spans="10:11">
+    <row r="21" spans="1:11">
       <c r="J21" t="s">
         <v>478</v>
       </c>
       <c r="K21" t="s">
         <v>479</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>480</v>
+      </c>
+      <c r="C23" t="s">
+        <v>481</v>
+      </c>
+      <c r="D23" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="C24" t="s">
+        <v>482</v>
+      </c>
+      <c r="D24" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="C25" t="s">
+        <v>484</v>
+      </c>
+      <c r="D25" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="C27" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="C28" t="s">
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -4952,7 +5003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63752E21-50CB-4B23-8BB5-9505E3D6C816}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
@@ -5692,7 +5743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B019C195-3E7A-4EF2-BB4B-1128AF09E9D2}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView topLeftCell="C13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changes to THC EXT A-D
</commit_message>
<xml_diff>
--- a/Hardware/Main Board/BOM LCSC.xlsx
+++ b/Hardware/Main Board/BOM LCSC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Main Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52165D3-78CD-4B9A-92D7-9BB6C2C6CD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C9C17A-1455-45F1-8031-3433F44B8127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42330" yWindow="5340" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="38280" yWindow="3360" windowWidth="29040" windowHeight="15840" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="503">
   <si>
     <t>Package</t>
   </si>
@@ -1536,13 +1536,300 @@
   </si>
   <si>
     <t>V1.2</t>
+  </si>
+  <si>
+    <t>;begin probe for ITH. THT=10.6mm</t>
+  </si>
+  <si>
+    <r>
+      <t>G21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC586C0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>G91</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (metric and relative)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>G38.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Z-35</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>F800</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (probe fast from safe retract, 24mm+THT)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>G1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Z12.6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (fast retract 2mm+THT)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>G38.2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Z-14.6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>F400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (slow probe max -2mm -last retract)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>G1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Z13.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>F800</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (fast retract to ITH, 2.5mm+THT, 150%-200% of cut height)</t>
+    </r>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <r>
+      <t>G4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>P1.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (pierce delay, THC delay s/b this+1.0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>G1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4EC9B0"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>F3400</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (restore feed rate and move mode)</t>
+    </r>
+  </si>
+  <si>
+    <t>;end probe ITH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1583,6 +1870,42 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC586C0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4EC9B0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDCDCAA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1685,7 +2008,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1734,6 +2057,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3273,10 +3605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C39F3-7594-4535-810B-0496FC455A11}">
-  <dimension ref="B1:O96"/>
+  <dimension ref="B1:P96"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="N68" sqref="N68"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3297,7 +3629,7 @@
     <col min="14" max="14" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:16">
       <c r="I1" s="17"/>
       <c r="J1" s="18"/>
       <c r="K1" s="17"/>
@@ -3306,7 +3638,7 @@
       <c r="N1" s="17"/>
       <c r="O1" s="17"/>
     </row>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:16">
       <c r="I2" s="17"/>
       <c r="J2" s="18"/>
       <c r="K2" s="17"/>
@@ -3315,7 +3647,7 @@
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:16">
       <c r="I3" s="17"/>
       <c r="J3" s="18"/>
       <c r="K3" s="17"/>
@@ -3324,7 +3656,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:16">
       <c r="B4" t="s">
         <v>138</v>
       </c>
@@ -3360,7 +3692,7 @@
       </c>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:16">
       <c r="I5" s="17"/>
       <c r="J5" s="18"/>
       <c r="K5" s="17"/>
@@ -3369,7 +3701,7 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:16">
       <c r="B6" t="s">
         <v>139</v>
       </c>
@@ -3382,8 +3714,11 @@
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
       <c r="O6" s="17"/>
-    </row>
-    <row r="7" spans="2:15">
+      <c r="P6" s="31" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
       <c r="B7" t="s">
         <v>140</v>
       </c>
@@ -3398,8 +3733,11 @@
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
       <c r="O7" s="17"/>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="P7" s="32" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
       <c r="B8" t="s">
         <v>156</v>
       </c>
@@ -3426,8 +3764,11 @@
       <c r="M8" s="19"/>
       <c r="N8" s="19"/>
       <c r="O8" s="17"/>
-    </row>
-    <row r="9" spans="2:15">
+      <c r="P8" s="32" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
       <c r="B9" t="s">
         <v>144</v>
       </c>
@@ -3442,8 +3783,11 @@
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
       <c r="O9" s="17"/>
-    </row>
-    <row r="10" spans="2:15">
+      <c r="P9" s="32" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
       <c r="B10" t="s">
         <v>158</v>
       </c>
@@ -3470,8 +3814,11 @@
       <c r="M10" s="19"/>
       <c r="N10" s="19"/>
       <c r="O10" s="17"/>
-    </row>
-    <row r="11" spans="2:15">
+      <c r="P10" s="32" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
       <c r="B11" t="s">
         <v>150</v>
       </c>
@@ -3506,8 +3853,11 @@
         <v>169</v>
       </c>
       <c r="O11" s="17"/>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="P11" s="32" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
       <c r="B12" t="s">
         <v>441</v>
       </c>
@@ -3545,8 +3895,11 @@
         <v>171</v>
       </c>
       <c r="O12" s="17"/>
-    </row>
-    <row r="13" spans="2:15">
+      <c r="P12" s="33" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
       <c r="B13" t="s">
         <v>155</v>
       </c>
@@ -3570,8 +3923,11 @@
         <v>172</v>
       </c>
       <c r="O13" s="17"/>
-    </row>
-    <row r="14" spans="2:15">
+      <c r="P13" s="32" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
       <c r="B14" t="s">
         <v>193</v>
       </c>
@@ -3595,8 +3951,11 @@
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
       <c r="O14" s="17"/>
-    </row>
-    <row r="15" spans="2:15">
+      <c r="P14" s="32" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
       <c r="B15" t="s">
         <v>443</v>
       </c>
@@ -3624,8 +3983,11 @@
       </c>
       <c r="N15" s="19"/>
       <c r="O15" s="17"/>
-    </row>
-    <row r="16" spans="2:15">
+      <c r="P15" s="31" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
       <c r="B16" t="s">
         <v>219</v>
       </c>
@@ -4785,7 +5147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68E6E9A4-984E-47E0-AB78-3A5B51A2C28B}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>